<commit_message>
update wetland depth data
</commit_message>
<xml_diff>
--- a/Wetlands/WetlandDepths.xlsx
+++ b/Wetlands/WetlandDepths.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Wetlands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BFB655-1689-804F-9510-ADC67EE06539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B97E235-BE7B-E840-AD62-B5AEA4BFC3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{F40B5C83-C7BF-4448-8AC9-BF76475CEB57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="13">
   <si>
     <t>Transect</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Wetland_08</t>
+  </si>
+  <si>
+    <t>Wetland_11</t>
+  </si>
+  <si>
+    <t>Wetland_10</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11EA31E-2127-8143-8D18-33FE489B28C2}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1643,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B86" s="1">
         <v>0.59375</v>
@@ -1651,7 +1657,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B87" s="1">
         <v>0.59375</v>
@@ -1665,7 +1671,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B88" s="1">
         <v>0.59375</v>
@@ -1675,6 +1681,258 @@
       </c>
       <c r="D88">
         <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+      <c r="D105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on water level data
</commit_message>
<xml_diff>
--- a/Wetlands/WetlandDepths.xlsx
+++ b/Wetlands/WetlandDepths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Wetlands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC251C53-3BFA-D845-8E30-D93181CCE4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B9CACB-189D-EC4F-B6EC-CAB608F6088F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="11160" windowHeight="17440" xr2:uid="{F40B5C83-C7BF-4448-8AC9-BF76475CEB57}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="16">
   <si>
     <t>Transect</t>
   </si>
@@ -79,6 +79,12 @@
   <si>
     <t>Wetland_05</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Wetland_09</t>
+  </si>
 </sst>
 </file>
 
@@ -119,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,1632 +443,2028 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11EA31E-2127-8143-8D18-33FE489B28C2}">
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B115" sqref="A107:B115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <f>35.6+0.4</f>
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <f>40.8+0.4</f>
         <v>41.199999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <f>100.1+0.4</f>
         <v>100.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <f>100.27+0.4</f>
         <v>100.67</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <f>100.1+0.4</f>
         <v>100.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
       <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <f>73+36</f>
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
       <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
         <f>85+36</f>
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
       <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
         <f>100+36</f>
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C10" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
       <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
         <f>72+36</f>
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
       <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
         <f>43+36</f>
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
       <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C13" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
       <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
       <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
       <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
       <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
       <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C18" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
       <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C19" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
       <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C20" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
       <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C21" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
       <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C22" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C23" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C24" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>5</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C25" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C26" s="1">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C27" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
       <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C28" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
       <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C29" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
       <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
         <v>20.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C30" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
       <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C31" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
       <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C32" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
       <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C33" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
       <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C34" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
       <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C35" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
       <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C36" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
       <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C37" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
       <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C38" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
       <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C39" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
       <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C40" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
       <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C41" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
       <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C42" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
       <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C43" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
       <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C44" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C44">
-        <v>4</v>
-      </c>
       <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C45" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
       <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C46" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
       <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C47" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
       <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C48" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
       <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C49" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C50" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
       <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C51" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
       <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C52" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
       <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C53" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C53">
-        <v>3</v>
-      </c>
       <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C54" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
       <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C55" s="1">
         <v>0.53125</v>
       </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
       <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C56" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
       <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C57" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
       <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C58" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
       <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C59" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
       <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C60" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
       <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C61" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
       <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C62" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C62">
-        <v>3</v>
-      </c>
       <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C63" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C63">
-        <v>3</v>
-      </c>
       <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C64" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C64">
-        <v>3</v>
-      </c>
       <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C65" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
       <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C66" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
       <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C67" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
       <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
         <v>28.1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C68" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
       <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
         <v>26.6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C69" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
       <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C70" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
       <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C71" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C71">
-        <v>3</v>
-      </c>
       <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C72" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
       <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C73" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C73">
-        <v>3</v>
-      </c>
       <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C74" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
       <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C75" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
       <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>9</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C76" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
       <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C77" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
       <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
         <v>23.8</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C78" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
       <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C79" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
       <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
         <v>25.8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>9</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C80" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
       <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
         <v>15.6</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C81" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C81">
-        <v>3</v>
-      </c>
       <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C82" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C82">
-        <v>3</v>
-      </c>
       <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C83" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C83">
-        <v>4</v>
-      </c>
       <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C84" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C84">
-        <v>4</v>
-      </c>
       <c r="D84">
+        <v>4</v>
+      </c>
+      <c r="E84">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C85" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C85">
-        <v>4</v>
-      </c>
       <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C86" s="1">
         <v>0.59375</v>
       </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
       <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C87" s="1">
         <v>0.59375</v>
       </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
       <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
+        <v>45097</v>
+      </c>
+      <c r="C88" s="1">
         <v>0.59375</v>
       </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
       <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C89" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
       <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C90" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
       <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C91" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
       <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>10</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C92" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C92">
-        <v>2</v>
-      </c>
       <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>10</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C93" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
       <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>10</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C94" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
       <c r="D94">
+        <v>2</v>
+      </c>
+      <c r="E94">
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C95" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C95">
-        <v>3</v>
-      </c>
       <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95">
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>10</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C96" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C96">
-        <v>3</v>
-      </c>
       <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96">
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C97" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C97">
-        <v>3</v>
-      </c>
       <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C98" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
       <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C99" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
       <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C100" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C100">
-        <v>1</v>
-      </c>
       <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C101" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C101">
-        <v>2</v>
-      </c>
       <c r="D101">
+        <v>2</v>
+      </c>
+      <c r="E101">
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C102" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C102">
-        <v>2</v>
-      </c>
       <c r="D102">
+        <v>2</v>
+      </c>
+      <c r="E102">
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C103" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C103">
-        <v>2</v>
-      </c>
       <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103">
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C104" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C104">
-        <v>3</v>
-      </c>
       <c r="D104">
+        <v>3</v>
+      </c>
+      <c r="E104">
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C105" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C105">
-        <v>3</v>
-      </c>
       <c r="D105">
+        <v>3</v>
+      </c>
+      <c r="E105">
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>12</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C106" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C106">
-        <v>3</v>
-      </c>
       <c r="D106">
+        <v>3</v>
+      </c>
+      <c r="E106">
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>13</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C107" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
       <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
         <v>35</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>13</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C108" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
       <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
         <v>47</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>13</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C109" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
       <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>13</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C110" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C110">
-        <v>2</v>
-      </c>
       <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110">
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>13</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C111" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C111">
-        <v>2</v>
-      </c>
       <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111">
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>13</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C112" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C112">
-        <v>2</v>
-      </c>
       <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112">
         <v>61</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>13</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C113" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C113">
-        <v>3</v>
-      </c>
       <c r="D113">
+        <v>3</v>
+      </c>
+      <c r="E113">
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>13</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C114" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C114">
-        <v>3</v>
-      </c>
       <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114">
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>13</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="2">
+        <v>45163</v>
+      </c>
+      <c r="C115" s="1">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C115">
-        <v>3</v>
-      </c>
       <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115">
         <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>15</v>
+      </c>
+      <c r="B117" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>15</v>
+      </c>
+      <c r="B118" s="2">
+        <v>45127</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>